<commit_message>
3.0.4: Implement JsonCreator option. Enable alias for field list.
</commit_message>
<xml_diff>
--- a/meta/objects2/BlancoValueObjectExtendedClass.xlsx
+++ b/meta/objects2/BlancoValueObjectExtendedClass.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10A7E09-3719-1641-874B-B269F66FBE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8C446B-02CD-434F-9A66-D1685B333A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="12820" windowWidth="28880" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="12900" windowWidth="28880" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
   <si>
     <t>クラス名</t>
   </si>
@@ -306,12 +306,95 @@
     <t>パッケージ</t>
     <phoneticPr fontId="3"/>
   </si>
+  <si>
+    <t>アノテーション(Kt)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>@Introspected
+@Serdeable</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>JsonCreatorを指定</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>/* kotlin 独自, primary constructor に @JsonCreator を指定する。コンストラクタ引数には @JsonProperty を自動付与する（別名優先）。 */</t>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">ドクジ </t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t xml:space="preserve">シテイスル </t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t xml:space="preserve">ヒキスウ </t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t xml:space="preserve">ジドウ </t>
+    </rPh>
+    <rPh sb="84" eb="86">
+      <t xml:space="preserve">フヨ </t>
+    </rPh>
+    <rPh sb="89" eb="91">
+      <t xml:space="preserve">ベツメイ </t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t xml:space="preserve">ユウセｎ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>field1</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>インタフェース名</t>
+    <rPh sb="0" eb="8">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>インポートクラス名</t>
+    <rPh sb="8" eb="9">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>バリューオブジェクト定義(php)・実装</t>
+    <rPh sb="18" eb="20">
+      <t xml:space="preserve">ジッソウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>バリューオブジェクト定義(php)・インポート</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>io.micronaut.core.annotation.Introspected</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>com.fasterxml.jackson.annotation.*</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>io.micronaut.serde.annotation.Serdeable</t>
+    <phoneticPr fontId="4"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -341,6 +424,13 @@
       <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="2"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -382,7 +472,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -852,11 +942,111 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -951,6 +1141,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -981,21 +1183,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1406,10 +1626,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1481,79 +1701,60 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="O8" s="52"/>
+    </row>
+    <row r="9" spans="1:17" ht="30">
+      <c r="A9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="45"/>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="3" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="45"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="45"/>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-      <c r="N11"/>
-      <c r="O11"/>
-      <c r="P11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="45"/>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="36" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="37" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -1571,7 +1772,7 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="36" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="37" t="s">
@@ -1592,10 +1793,16 @@
       <c r="P13"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="65"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="66"/>
-      <c r="D14"/>
+      <c r="A14" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
@@ -1610,9 +1817,13 @@
       <c r="P14"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
+      <c r="A15" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="37" t="s">
+        <v>23</v>
+      </c>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
@@ -1628,417 +1839,781 @@
       <c r="P15"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+    </row>
+    <row r="17" spans="1:25">
+      <c r="A17" s="54"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="55"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+    </row>
+    <row r="18" spans="1:25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+    </row>
+    <row r="19" spans="1:25">
+      <c r="A19" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="46"/>
-    </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="31" t="s">
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="46"/>
+    </row>
+    <row r="20" spans="1:25">
+      <c r="A20" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="33" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="48"/>
-    </row>
-    <row r="18" spans="1:18">
-      <c r="A18" s="3" t="s">
+      <c r="D20" s="33"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="A21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="9" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="48"/>
-      <c r="O18" s="48"/>
-    </row>
-    <row r="19" spans="1:18">
-      <c r="A19" s="60"/>
-      <c r="B19" s="61"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="48"/>
-      <c r="O19" s="48"/>
-    </row>
-    <row r="20" spans="1:18">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
-      <c r="O20"/>
-      <c r="P20"/>
-    </row>
-    <row r="21" spans="1:18">
-      <c r="A21" s="3" t="s">
+      <c r="D21" s="33"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
+    </row>
+    <row r="22" spans="1:25">
+      <c r="A22" s="50"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+    </row>
+    <row r="23" spans="1:25">
+      <c r="A23" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+    </row>
+    <row r="24" spans="1:25">
+      <c r="A24" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="48"/>
+      <c r="P24" s="48"/>
+      <c r="Q24" s="48"/>
+      <c r="R24" s="48"/>
+      <c r="S24" s="48"/>
+      <c r="T24" s="48"/>
+      <c r="U24" s="48"/>
+      <c r="V24" s="48"/>
+      <c r="X24" s="67"/>
+      <c r="Y24" s="67"/>
+    </row>
+    <row r="25" spans="1:25">
+      <c r="A25" s="71"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="68"/>
+      <c r="L25" s="68"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="68"/>
+      <c r="O25" s="68"/>
+      <c r="P25" s="68"/>
+      <c r="Q25" s="68"/>
+      <c r="R25" s="68"/>
+      <c r="S25" s="68"/>
+      <c r="T25" s="68"/>
+      <c r="U25" s="68"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+    </row>
+    <row r="26" spans="1:25">
+      <c r="A26" s="71"/>
+      <c r="B26" s="72"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="68"/>
+      <c r="L26" s="68"/>
+      <c r="M26" s="68"/>
+      <c r="N26" s="68"/>
+      <c r="O26" s="68"/>
+      <c r="P26" s="68"/>
+      <c r="Q26" s="68"/>
+      <c r="R26" s="68"/>
+      <c r="S26" s="68"/>
+      <c r="T26" s="68"/>
+      <c r="U26" s="68"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26"/>
+    </row>
+    <row r="27" spans="1:25">
+      <c r="A27" s="77"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="68"/>
+      <c r="M27" s="68"/>
+      <c r="N27" s="68"/>
+      <c r="O27" s="68"/>
+      <c r="P27" s="68"/>
+      <c r="Q27" s="68"/>
+      <c r="R27" s="68"/>
+      <c r="S27" s="68"/>
+      <c r="T27" s="68"/>
+      <c r="U27" s="68"/>
+      <c r="W27"/>
+      <c r="X27"/>
+      <c r="Y27"/>
+    </row>
+    <row r="28" spans="1:25">
+      <c r="B28"/>
+    </row>
+    <row r="29" spans="1:25">
+      <c r="A29" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+    </row>
+    <row r="30" spans="1:25">
+      <c r="A30" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="70"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="48"/>
+      <c r="P30" s="48"/>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="48"/>
+      <c r="S30" s="48"/>
+      <c r="T30" s="48"/>
+      <c r="U30" s="48"/>
+      <c r="V30" s="48"/>
+      <c r="X30" s="67"/>
+      <c r="Y30" s="67"/>
+    </row>
+    <row r="31" spans="1:25">
+      <c r="A31" s="71">
+        <v>1</v>
+      </c>
+      <c r="B31" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="68"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="68"/>
+      <c r="O31" s="68"/>
+      <c r="P31" s="68"/>
+      <c r="Q31" s="68"/>
+      <c r="R31" s="68"/>
+      <c r="S31" s="68"/>
+      <c r="T31" s="68"/>
+      <c r="U31" s="68"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+    </row>
+    <row r="32" spans="1:25">
+      <c r="A32" s="71">
+        <f>A31+1</f>
+        <v>2</v>
+      </c>
+      <c r="B32" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="76"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="68"/>
+      <c r="N32" s="68"/>
+      <c r="O32" s="68"/>
+      <c r="P32" s="68"/>
+      <c r="Q32" s="68"/>
+      <c r="R32" s="68"/>
+      <c r="S32" s="68"/>
+      <c r="T32" s="68"/>
+      <c r="U32" s="68"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Y32"/>
+    </row>
+    <row r="33" spans="1:25">
+      <c r="A33" s="71">
+        <f>A32+1</f>
+        <v>3</v>
+      </c>
+      <c r="B33" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="81"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="82"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="68"/>
+      <c r="J33" s="68"/>
+      <c r="K33" s="68"/>
+      <c r="L33" s="68"/>
+      <c r="M33" s="68"/>
+      <c r="N33" s="68"/>
+      <c r="O33" s="68"/>
+      <c r="P33" s="68"/>
+      <c r="Q33" s="68"/>
+      <c r="R33" s="68"/>
+      <c r="S33" s="68"/>
+      <c r="T33" s="68"/>
+      <c r="U33" s="68"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="Y33"/>
+    </row>
+    <row r="34" spans="1:25">
+      <c r="A34" s="77"/>
+      <c r="B34" s="78"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="79"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="68"/>
+      <c r="J34" s="68"/>
+      <c r="K34" s="68"/>
+      <c r="L34" s="68"/>
+      <c r="M34" s="68"/>
+      <c r="N34" s="68"/>
+      <c r="O34" s="68"/>
+      <c r="P34" s="68"/>
+      <c r="Q34" s="68"/>
+      <c r="R34" s="68"/>
+      <c r="S34" s="68"/>
+      <c r="T34" s="68"/>
+      <c r="U34" s="68"/>
+      <c r="W34"/>
+      <c r="X34"/>
+      <c r="Y34"/>
+    </row>
+    <row r="35" spans="1:25">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+    </row>
+    <row r="36" spans="1:25">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+    </row>
+    <row r="37" spans="1:25">
+      <c r="A37" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="6"/>
-    </row>
-    <row r="22" spans="1:18" ht="13.5" customHeight="1">
-      <c r="A22" s="51" t="s">
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="12"/>
+      <c r="Q37" s="12"/>
+      <c r="R37" s="6"/>
+    </row>
+    <row r="38" spans="1:25" ht="13.5" customHeight="1">
+      <c r="A38" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B38" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C38" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="50" t="s">
+      <c r="D38" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="50" t="s">
+      <c r="E38" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="50" t="s">
+      <c r="F38" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="52" t="s">
+      <c r="G38" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="54" t="s">
+      <c r="H38" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="I22" s="58" t="s">
+      <c r="I38" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="J22" s="56" t="s">
+      <c r="J38" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="K22" s="56" t="s">
+      <c r="K38" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="56" t="s">
+      <c r="L38" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="M22" s="56" t="s">
+      <c r="M38" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="N22" s="56" t="s">
+      <c r="N38" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="O22" s="50" t="s">
+      <c r="O38" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="P22" s="50"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="14"/>
-    </row>
-    <row r="23" spans="1:18">
-      <c r="A23" s="51"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="57"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="57"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="27"/>
-    </row>
-    <row r="24" spans="1:18">
-      <c r="A24" s="16">
+      <c r="P38" s="56"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="14"/>
+    </row>
+    <row r="39" spans="1:25">
+      <c r="A39" s="57"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="59"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="65"/>
+      <c r="J39" s="63"/>
+      <c r="K39" s="63"/>
+      <c r="L39" s="63"/>
+      <c r="M39" s="63"/>
+      <c r="N39" s="63"/>
+      <c r="O39" s="56"/>
+      <c r="P39" s="56"/>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="27"/>
+    </row>
+    <row r="40" spans="1:25">
+      <c r="A40" s="16">
         <v>1</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B40" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C40" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="49" t="s">
+      <c r="D40" s="18"/>
+      <c r="E40" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F40" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18" t="s">
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="N24" s="18" t="s">
+      <c r="N40" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="O24" s="18" t="s">
+      <c r="O40" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="26"/>
-    </row>
-    <row r="25" spans="1:18">
-      <c r="A25" s="16">
-        <f>A24+1</f>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="26"/>
+    </row>
+    <row r="41" spans="1:25">
+      <c r="A41" s="16">
+        <f>A40+1</f>
         <v>2</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B41" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C41" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="49" t="s">
+      <c r="D41" s="18"/>
+      <c r="E41" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="18" t="s">
+      <c r="F41" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18" t="s">
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="N25" s="18" t="s">
+      <c r="N41" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="O25" s="18" t="s">
+      <c r="O41" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="20"/>
-    </row>
-    <row r="26" spans="1:18">
-      <c r="A26" s="16">
-        <f t="shared" ref="A26:A27" si="0">A25+1</f>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="20"/>
+    </row>
+    <row r="42" spans="1:25">
+      <c r="A42" s="16">
+        <f t="shared" ref="A42:A43" si="0">A41+1</f>
         <v>3</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B42" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C42" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="49" t="s">
+      <c r="D42" s="18"/>
+      <c r="E42" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F42" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18" t="s">
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="O26" s="18"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="20"/>
-    </row>
-    <row r="27" spans="1:18">
-      <c r="A27" s="16">
+      <c r="O42" s="18"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="20"/>
+    </row>
+    <row r="43" spans="1:25">
+      <c r="A43" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B43" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C43" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="49" t="s">
+      <c r="D43" s="18"/>
+      <c r="E43" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F43" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18" t="s">
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="O27" s="18"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="20"/>
-    </row>
-    <row r="28" spans="1:18">
-      <c r="A28" s="16"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="20"/>
-    </row>
-    <row r="29" spans="1:18">
-      <c r="A29" s="16"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="20"/>
-    </row>
-    <row r="30" spans="1:18">
-      <c r="A30" s="21"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="25"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="20"/>
+    </row>
+    <row r="44" spans="1:25">
+      <c r="A44" s="16"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="20"/>
+    </row>
+    <row r="45" spans="1:25">
+      <c r="A45" s="16"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="19"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="20"/>
+    </row>
+    <row r="46" spans="1:25">
+      <c r="A46" s="21"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="23"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="23"/>
+      <c r="O46" s="23"/>
+      <c r="P46" s="24"/>
+      <c r="Q46" s="24"/>
+      <c r="R46" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="O22:P23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="O38:P39"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="M38:M39"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E46:N46" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E62:N62" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:C14" xr:uid="{9B350086-4234-7F42-90E1-E9696B21763F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16:C17" xr:uid="{9B350086-4234-7F42-90E1-E9696B21763F}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C12" xr:uid="{37676737-95C3-434E-BC4C-270691A9AC5F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:C15" xr:uid="{37676737-95C3-434E-BC4C-270691A9AC5F}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{7083602A-A73F-BE48-A359-8D659B03A9B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{7083602A-A73F-BE48-A359-8D659B03A9B3}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G24:N30" xr:uid="{DC9EBF38-7703-0D4E-BA7E-C817D1AB0B2C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G40:J46 L40:N46" xr:uid="{DC9EBF38-7703-0D4E-BA7E-C817D1AB0B2C}">
       <formula1>isAbstract</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
3.0.10: Add @Nullable annotation if Required option is not specified.
</commit_message>
<xml_diff>
--- a/meta/objects2/BlancoValueObjectExtendedClass.xlsx
+++ b/meta/objects2/BlancoValueObjectExtendedClass.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8C446B-02CD-434F-9A66-D1685B333A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA157ADB-7811-D741-A9EF-E2BAE2BF3DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="12900" windowWidth="28880" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
   <si>
     <t>クラス名</t>
   </si>
@@ -222,10 +222,6 @@
   </si>
   <si>
     <t>アノテーション</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>@field:NotNull</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -1153,36 +1149,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1216,6 +1182,36 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1628,8 +1624,8 @@
   </sheetPr>
   <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1681,7 +1677,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="8"/>
@@ -1714,11 +1710,11 @@
     </row>
     <row r="9" spans="1:17" ht="30">
       <c r="A9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="56" t="s">
         <v>55</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="66" t="s">
-        <v>56</v>
       </c>
       <c r="D9" s="35"/>
       <c r="E9" s="35"/>
@@ -1794,14 +1790,14 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="37" t="s">
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
@@ -1929,7 +1925,7 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="9" t="s">
@@ -1967,7 +1963,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -1976,15 +1972,15 @@
       <c r="F23" s="29"/>
     </row>
     <row r="24" spans="1:25">
-      <c r="A24" s="69" t="s">
+      <c r="A24" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="70" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
       <c r="F24" s="32"/>
       <c r="G24" s="48"/>
       <c r="H24" s="48"/>
@@ -2002,83 +1998,83 @@
       <c r="T24" s="48"/>
       <c r="U24" s="48"/>
       <c r="V24" s="48"/>
-      <c r="X24" s="67"/>
-      <c r="Y24" s="67"/>
+      <c r="X24" s="57"/>
+      <c r="Y24" s="57"/>
     </row>
     <row r="25" spans="1:25">
-      <c r="A25" s="71"/>
-      <c r="B25" s="72"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="68"/>
-      <c r="L25" s="68"/>
-      <c r="M25" s="68"/>
-      <c r="N25" s="68"/>
-      <c r="O25" s="68"/>
-      <c r="P25" s="68"/>
-      <c r="Q25" s="68"/>
-      <c r="R25" s="68"/>
-      <c r="S25" s="68"/>
-      <c r="T25" s="68"/>
-      <c r="U25" s="68"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="58"/>
+      <c r="Q25" s="58"/>
+      <c r="R25" s="58"/>
+      <c r="S25" s="58"/>
+      <c r="T25" s="58"/>
+      <c r="U25" s="58"/>
       <c r="W25"/>
       <c r="X25"/>
       <c r="Y25"/>
     </row>
     <row r="26" spans="1:25">
-      <c r="A26" s="71"/>
-      <c r="B26" s="72"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="76"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="68"/>
-      <c r="L26" s="68"/>
-      <c r="M26" s="68"/>
-      <c r="N26" s="68"/>
-      <c r="O26" s="68"/>
-      <c r="P26" s="68"/>
-      <c r="Q26" s="68"/>
-      <c r="R26" s="68"/>
-      <c r="S26" s="68"/>
-      <c r="T26" s="68"/>
-      <c r="U26" s="68"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="58"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="58"/>
+      <c r="N26" s="58"/>
+      <c r="O26" s="58"/>
+      <c r="P26" s="58"/>
+      <c r="Q26" s="58"/>
+      <c r="R26" s="58"/>
+      <c r="S26" s="58"/>
+      <c r="T26" s="58"/>
+      <c r="U26" s="58"/>
       <c r="W26"/>
       <c r="X26"/>
       <c r="Y26"/>
     </row>
     <row r="27" spans="1:25">
-      <c r="A27" s="77"/>
-      <c r="B27" s="78"/>
-      <c r="C27" s="79"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="80"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="68"/>
-      <c r="L27" s="68"/>
-      <c r="M27" s="68"/>
-      <c r="N27" s="68"/>
-      <c r="O27" s="68"/>
-      <c r="P27" s="68"/>
-      <c r="Q27" s="68"/>
-      <c r="R27" s="68"/>
-      <c r="S27" s="68"/>
-      <c r="T27" s="68"/>
-      <c r="U27" s="68"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="58"/>
+      <c r="J27" s="58"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="58"/>
+      <c r="N27" s="58"/>
+      <c r="O27" s="58"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="58"/>
+      <c r="R27" s="58"/>
+      <c r="S27" s="58"/>
+      <c r="T27" s="58"/>
+      <c r="U27" s="58"/>
       <c r="W27"/>
       <c r="X27"/>
       <c r="Y27"/>
@@ -2088,7 +2084,7 @@
     </row>
     <row r="29" spans="1:25">
       <c r="A29" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
@@ -2097,15 +2093,15 @@
       <c r="F29" s="29"/>
     </row>
     <row r="30" spans="1:25">
-      <c r="A30" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="70" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
+      <c r="A30" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
       <c r="F30" s="32"/>
       <c r="G30" s="48"/>
       <c r="H30" s="48"/>
@@ -2123,123 +2119,123 @@
       <c r="T30" s="48"/>
       <c r="U30" s="48"/>
       <c r="V30" s="48"/>
-      <c r="X30" s="67"/>
-      <c r="Y30" s="67"/>
+      <c r="X30" s="57"/>
+      <c r="Y30" s="57"/>
     </row>
     <row r="31" spans="1:25">
-      <c r="A31" s="71">
+      <c r="A31" s="61">
         <v>1</v>
       </c>
-      <c r="B31" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="68"/>
-      <c r="K31" s="68"/>
-      <c r="L31" s="68"/>
-      <c r="M31" s="68"/>
-      <c r="N31" s="68"/>
-      <c r="O31" s="68"/>
-      <c r="P31" s="68"/>
-      <c r="Q31" s="68"/>
-      <c r="R31" s="68"/>
-      <c r="S31" s="68"/>
-      <c r="T31" s="68"/>
-      <c r="U31" s="68"/>
+      <c r="B31" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="63"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="58"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="58"/>
+      <c r="P31" s="58"/>
+      <c r="Q31" s="58"/>
+      <c r="R31" s="58"/>
+      <c r="S31" s="58"/>
+      <c r="T31" s="58"/>
+      <c r="U31" s="58"/>
       <c r="W31"/>
       <c r="X31"/>
       <c r="Y31"/>
     </row>
     <row r="32" spans="1:25">
-      <c r="A32" s="71">
+      <c r="A32" s="61">
         <f>A31+1</f>
         <v>2</v>
       </c>
-      <c r="B32" s="72" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="76"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="68"/>
-      <c r="L32" s="68"/>
-      <c r="M32" s="68"/>
-      <c r="N32" s="68"/>
-      <c r="O32" s="68"/>
-      <c r="P32" s="68"/>
-      <c r="Q32" s="68"/>
-      <c r="R32" s="68"/>
-      <c r="S32" s="68"/>
-      <c r="T32" s="68"/>
-      <c r="U32" s="68"/>
+      <c r="B32" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="58"/>
+      <c r="J32" s="58"/>
+      <c r="K32" s="58"/>
+      <c r="L32" s="58"/>
+      <c r="M32" s="58"/>
+      <c r="N32" s="58"/>
+      <c r="O32" s="58"/>
+      <c r="P32" s="58"/>
+      <c r="Q32" s="58"/>
+      <c r="R32" s="58"/>
+      <c r="S32" s="58"/>
+      <c r="T32" s="58"/>
+      <c r="U32" s="58"/>
       <c r="W32"/>
       <c r="X32"/>
       <c r="Y32"/>
     </row>
     <row r="33" spans="1:25">
-      <c r="A33" s="71">
+      <c r="A33" s="61">
         <f>A32+1</f>
         <v>3</v>
       </c>
-      <c r="B33" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="82"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="68"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="68"/>
-      <c r="L33" s="68"/>
-      <c r="M33" s="68"/>
-      <c r="N33" s="68"/>
-      <c r="O33" s="68"/>
-      <c r="P33" s="68"/>
-      <c r="Q33" s="68"/>
-      <c r="R33" s="68"/>
-      <c r="S33" s="68"/>
-      <c r="T33" s="68"/>
-      <c r="U33" s="68"/>
+      <c r="B33" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="72"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="58"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="58"/>
+      <c r="M33" s="58"/>
+      <c r="N33" s="58"/>
+      <c r="O33" s="58"/>
+      <c r="P33" s="58"/>
+      <c r="Q33" s="58"/>
+      <c r="R33" s="58"/>
+      <c r="S33" s="58"/>
+      <c r="T33" s="58"/>
+      <c r="U33" s="58"/>
       <c r="W33"/>
       <c r="X33"/>
       <c r="Y33"/>
     </row>
     <row r="34" spans="1:25">
-      <c r="A34" s="77"/>
-      <c r="B34" s="78"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="79"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="80"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="68"/>
-      <c r="K34" s="68"/>
-      <c r="L34" s="68"/>
-      <c r="M34" s="68"/>
-      <c r="N34" s="68"/>
-      <c r="O34" s="68"/>
-      <c r="P34" s="68"/>
-      <c r="Q34" s="68"/>
-      <c r="R34" s="68"/>
-      <c r="S34" s="68"/>
-      <c r="T34" s="68"/>
-      <c r="U34" s="68"/>
+      <c r="A34" s="67"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="58"/>
+      <c r="J34" s="58"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="58"/>
+      <c r="M34" s="58"/>
+      <c r="N34" s="58"/>
+      <c r="O34" s="58"/>
+      <c r="P34" s="58"/>
+      <c r="Q34" s="58"/>
+      <c r="R34" s="58"/>
+      <c r="S34" s="58"/>
+      <c r="T34" s="58"/>
+      <c r="U34" s="58"/>
       <c r="W34"/>
       <c r="X34"/>
       <c r="Y34"/>
@@ -2310,72 +2306,72 @@
       <c r="R37" s="6"/>
     </row>
     <row r="38" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="57" t="s">
+      <c r="B38" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="56" t="s">
+      <c r="C38" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="56" t="s">
+      <c r="D38" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="E38" s="56" t="s">
+      <c r="E38" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="F38" s="56" t="s">
+      <c r="F38" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="G38" s="58" t="s">
+      <c r="G38" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="H38" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="H38" s="60" t="s">
+      <c r="I38" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="I38" s="64" t="s">
+      <c r="J38" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="J38" s="62" t="s">
+      <c r="K38" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="K38" s="62" t="s">
+      <c r="L38" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="L38" s="62" t="s">
+      <c r="M38" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="M38" s="62" t="s">
+      <c r="N38" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="N38" s="62" t="s">
-        <v>47</v>
-      </c>
-      <c r="O38" s="56" t="s">
+      <c r="O38" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="P38" s="56"/>
+      <c r="P38" s="73"/>
       <c r="Q38" s="13"/>
       <c r="R38" s="14"/>
     </row>
     <row r="39" spans="1:25">
-      <c r="A39" s="57"/>
-      <c r="B39" s="57"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="59"/>
-      <c r="H39" s="61"/>
-      <c r="I39" s="65"/>
-      <c r="J39" s="63"/>
-      <c r="K39" s="63"/>
-      <c r="L39" s="63"/>
-      <c r="M39" s="63"/>
-      <c r="N39" s="63"/>
-      <c r="O39" s="56"/>
-      <c r="P39" s="56"/>
+      <c r="A39" s="74"/>
+      <c r="B39" s="74"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="76"/>
+      <c r="H39" s="78"/>
+      <c r="I39" s="82"/>
+      <c r="J39" s="80"/>
+      <c r="K39" s="80"/>
+      <c r="L39" s="80"/>
+      <c r="M39" s="80"/>
+      <c r="N39" s="80"/>
+      <c r="O39" s="73"/>
+      <c r="P39" s="73"/>
       <c r="Q39" s="15"/>
       <c r="R39" s="27"/>
     </row>
@@ -2390,18 +2386,18 @@
         <v>17</v>
       </c>
       <c r="D40" s="18"/>
-      <c r="E40" s="49" t="s">
-        <v>39</v>
-      </c>
+      <c r="E40" s="49"/>
       <c r="F40" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
+      <c r="I40" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="J40" s="18"/>
       <c r="K40" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L40" s="18"/>
       <c r="M40" s="18" t="s">
@@ -2411,7 +2407,7 @@
         <v>23</v>
       </c>
       <c r="O40" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P40" s="19"/>
       <c r="Q40" s="19"/>
@@ -2429,15 +2425,17 @@
         <v>20</v>
       </c>
       <c r="D41" s="18"/>
-      <c r="E41" s="49" t="s">
-        <v>39</v>
-      </c>
+      <c r="E41" s="49"/>
       <c r="F41" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
+      <c r="H41" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I41" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="J41" s="18"/>
       <c r="K41" s="18"/>
       <c r="L41" s="18"/>
@@ -2448,7 +2446,7 @@
         <v>23</v>
       </c>
       <c r="O41" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P41" s="19"/>
       <c r="Q41" s="19"/>
@@ -2460,17 +2458,15 @@
         <v>3</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D42" s="18"/>
-      <c r="E42" s="49" t="s">
-        <v>39</v>
-      </c>
+      <c r="E42" s="49"/>
       <c r="F42" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G42" s="18"/>
       <c r="H42" s="18"/>
@@ -2493,20 +2489,20 @@
         <v>4</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D43" s="18"/>
-      <c r="E43" s="49" t="s">
-        <v>39</v>
-      </c>
+      <c r="E43" s="49"/>
       <c r="F43" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
+      <c r="H43" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="I43" s="18"/>
       <c r="J43" s="18"/>
       <c r="K43" s="18"/>

</xml_diff>

<commit_message>
3.0.11: Avoid duplicate of annotaions added automatic and sheet defined.
</commit_message>
<xml_diff>
--- a/meta/objects2/BlancoValueObjectExtendedClass.xlsx
+++ b/meta/objects2/BlancoValueObjectExtendedClass.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA157ADB-7811-D741-A9EF-E2BAE2BF3DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50A16C2-5CB3-8945-8584-F977B80C8396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="12900" windowWidth="28880" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="12880" windowWidth="28880" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
   <si>
     <t>クラス名</t>
   </si>
@@ -384,6 +384,10 @@
   <si>
     <t>io.micronaut.serde.annotation.Serdeable</t>
     <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>@field:NotNull</t>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
@@ -1625,7 +1629,7 @@
   <dimension ref="A1:Y46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2386,7 +2390,9 @@
         <v>17</v>
       </c>
       <c r="D40" s="18"/>
-      <c r="E40" s="49"/>
+      <c r="E40" s="49" t="s">
+        <v>67</v>
+      </c>
       <c r="F40" s="18" t="s">
         <v>47</v>
       </c>

</xml_diff>